<commit_message>
Test class name corrected
Corrected name of the test class for task 2 criteria
</commit_message>
<xml_diff>
--- a/project-phase-1-marking-guide.xlsx
+++ b/project-phase-1-marking-guide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/00047104/Dropbox/CITS5501-2025/project-spec-2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09668823-F0C9-304C-878D-BBD93B00E72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AF9A9A-93E7-6744-8ADD-B8075B4D13D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{A08706B5-E2B8-9646-A6FC-7AEAC5D7CA21}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17300" xr2:uid="{A08706B5-E2B8-9646-A6FC-7AEAC5D7CA21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,22 +73,22 @@
 Cogent rationale for excluding this task from the software quailty plan. (2 marks)</t>
   </si>
   <si>
-    <t xml:space="preserve">2.1 Relevant Junit test cases have been written (relevant cases but not too many) and *documented* in CheckDataTimeStringTest.java (2 marks)
+    <t>Team ID</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>Marker (initials)</t>
+  </si>
+  <si>
+    <t>Marking Criteria and indicative marks (see also https://cits5501.arranstewart.io/faq/#marking-rubric)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.1 Relevant Junit test cases have been written (relevant cases but not too many) and *documented* in  DateTimeCheckerTest.java  (2 marks)
 2.2 Pull requests show evidence of effective (but not excessive) review of the new code (2 marks)
 2.3 Description of the software quality assurance plan for this project is clear and concise (max 500 words). Includes links to the github repository demonstrating your plan in action. (3 marks)
 </t>
-  </si>
-  <si>
-    <t>Team ID</t>
-  </si>
-  <si>
-    <t>XX</t>
-  </si>
-  <si>
-    <t>Marker (initials)</t>
-  </si>
-  <si>
-    <t>Marking Criteria and indicative marks (see also https://cits5501.arranstewart.io/faq/#marking-rubric)</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -559,15 +559,15 @@
     </row>
     <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="5"/>
@@ -586,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>